<commit_message>
I have completed automation script for - > owners -> Rental Listings & Applications.
</commit_message>
<xml_diff>
--- a/TestData_Name_Pwd.xlsx
+++ b/TestData_Name_Pwd.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D26B90E-89EE-4BF0-9508-BCACD28C50B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE38437D-9246-4A41-9D79-276999210462}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>UserName</t>
   </si>
@@ -38,6 +39,42 @@
   </si>
   <si>
     <t>ntmv2682</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Listing Sydney Homes</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Listing my property for rental</t>
+  </si>
+  <si>
+    <t>Moving Cost</t>
+  </si>
+  <si>
+    <t>Target Rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furnishing </t>
+  </si>
+  <si>
+    <t>Available_Date</t>
+  </si>
+  <si>
+    <t>Ideal_Tenant</t>
+  </si>
+  <si>
+    <t>Occupants_Count</t>
+  </si>
+  <si>
+    <t>Two Beds and Sofa</t>
+  </si>
+  <si>
+    <t>Do not come late</t>
   </si>
 </sst>
 </file>
@@ -82,9 +119,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -366,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,9 +421,13 @@
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,8 +437,32 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -399,6 +471,18 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>4000</v>
       </c>
     </row>
   </sheetData>
@@ -407,4 +491,78 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5807953-4087-45D6-987E-68893A7FB0AB}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>4000</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43343</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>